<commit_message>
Updates to german course II
</commit_message>
<xml_diff>
--- a/01_Deutsch/korrelationstabelle.xlsx
+++ b/01_Deutsch/korrelationstabelle.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -393,138 +393,115 @@
           <t>3.</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>4.</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1.w</t>
-        </is>
-      </c>
-      <c r="B2">
-        <v>-0.02</v>
-      </c>
-      <c r="C2">
-        <v>0.7</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
+          <t>1.a</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>3.03</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>0.99</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>.49</t>
+        </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>1***</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0.08</t>
+          <t>.32**</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>0.03</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>0.25*</t>
+          <t>.39***</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2.a</t>
-        </is>
-      </c>
-      <c r="B3">
-        <v>0.03</v>
-      </c>
-      <c r="C3">
-        <v>0.99</v>
-      </c>
-      <c r="D3">
-        <v>0.49</v>
+          <t>2.b</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1.95</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>1.07</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>.55</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>.22***</t>
+        </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>1***</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>0.32**</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>0.39***</t>
+          <t>.29**</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>3.b</t>
-        </is>
-      </c>
-      <c r="B4">
-        <v>-0.05</v>
-      </c>
-      <c r="C4">
-        <v>1.07</v>
-      </c>
-      <c r="D4">
-        <v>0.55</v>
+          <t>3.c</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1.99</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>1.06</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>.47</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>.25***</t>
+        </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0.22***</t>
+          <t>.29***</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>1***</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>0.29**</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>4.c</t>
-        </is>
-      </c>
-      <c r="B5">
-        <v>-0.01</v>
-      </c>
-      <c r="C5">
-        <v>1.06</v>
-      </c>
-      <c r="D5">
-        <v>0.47</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>0.25***</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>0.29***</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>1***</t>
+          <t>-</t>
         </is>
       </c>
     </row>

</xml_diff>